<commit_message>
updated the GPIOalternateFunctionList excel sheet to show which pins are currently being used as well as the function they are being used for. Added alot more GPIO use to the system init file, still need to do interrupts and maybe one more thing before moving to the ADC and clock systems.
</commit_message>
<xml_diff>
--- a/docs/GPIOalternateFunctionList.xlsx
+++ b/docs/GPIOalternateFunctionList.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2A7E20F-99F9-4914-9E30-C72ED688347F}" xr6:coauthVersionLast="42" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6577709-9A30-4C78-9977-E51774435CE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,7 +211,7 @@
     <t>eUSCI B SPI mode CLK</t>
   </si>
   <si>
-    <t>Internaly timed to DVSS</t>
+    <t>Internaly tied to DVSS</t>
   </si>
   <si>
     <t>P2.3</t>
@@ -314,15 +314,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -330,12 +336,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -679,7 +697,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -715,10 +733,10 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
@@ -726,16 +744,16 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -762,24 +780,24 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -806,24 +824,24 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -850,24 +868,24 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -902,16 +920,16 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -943,16 +961,16 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -976,27 +994,27 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C29" t="s">
         <v>41</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1031,16 +1049,16 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1075,16 +1093,16 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" t="s">
+      <c r="A38" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="B38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1119,16 +1137,16 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="B42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1166,16 +1184,16 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" t="s">
+      <c r="A46" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="B46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1210,16 +1228,16 @@
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" t="s">
+      <c r="A50" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B50" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="B50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1251,16 +1269,16 @@
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" t="s">
+      <c r="A54" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B54" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="B54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1295,16 +1313,16 @@
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" t="s">
+      <c r="A58" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="B58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1339,16 +1357,16 @@
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" t="s">
+      <c r="A62" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B62" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="B62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1386,16 +1404,16 @@
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" t="s">
+      <c r="A66" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B66" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="B66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1430,16 +1448,16 @@
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" t="s">
+      <c r="A70" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="B70" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1474,16 +1492,16 @@
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" t="s">
+      <c r="A74" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B74" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="B74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1518,16 +1536,16 @@
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" t="s">
+      <c r="A78" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B78" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="B78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1562,16 +1580,16 @@
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" t="s">
+      <c r="A82" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B82" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="B82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1609,16 +1627,16 @@
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" t="s">
+      <c r="A86" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B86" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="B86" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1656,16 +1674,16 @@
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" t="s">
+      <c r="A90" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B90" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="B90" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1703,16 +1721,16 @@
       </c>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" t="s">
+      <c r="A94" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B94" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="B94" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1750,16 +1768,16 @@
       </c>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" t="s">
+      <c r="A98" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B98" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="B98" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1794,16 +1812,16 @@
       </c>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" t="s">
+      <c r="A102" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B102" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" t="s">
-        <v>6</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="B102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1838,16 +1856,16 @@
       </c>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" t="s">
+      <c r="A106" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B106" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" t="s">
-        <v>6</v>
-      </c>
-      <c r="D106" t="s">
+      <c r="B106" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1882,16 +1900,16 @@
       </c>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" t="s">
+      <c r="A110" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B110" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" t="s">
-        <v>6</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="B110" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1926,16 +1944,16 @@
       </c>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" t="s">
+      <c r="A114" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B114" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" t="s">
-        <v>6</v>
-      </c>
-      <c r="D114" t="s">
+      <c r="B114" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1973,16 +1991,16 @@
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" t="s">
+      <c r="A118" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B118" t="s">
-        <v>5</v>
-      </c>
-      <c r="C118" t="s">
-        <v>6</v>
-      </c>
-      <c r="D118" t="s">
+      <c r="B118" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2020,16 +2038,16 @@
       </c>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" t="s">
+      <c r="A122" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B122" t="s">
-        <v>5</v>
-      </c>
-      <c r="C122" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="B122" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2067,16 +2085,16 @@
       </c>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" t="s">
+      <c r="A126" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B126" t="s">
-        <v>5</v>
-      </c>
-      <c r="C126" t="s">
-        <v>6</v>
-      </c>
-      <c r="D126" t="s">
+      <c r="B126" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D126" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the port J pins to the excel selection sheet.
</commit_message>
<xml_diff>
--- a/docs/GPIOalternateFunctionList.xlsx
+++ b/docs/GPIOalternateFunctionList.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21506"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6577709-9A30-4C78-9977-E51774435CE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="480" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{622749EB-DCF6-4A66-B22A-7F7CAC1B9150}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="115">
   <si>
     <t>Pin</t>
   </si>
@@ -299,6 +299,75 @@
   </si>
   <si>
     <t>P4.7</t>
+  </si>
+  <si>
+    <t>PJ.0</t>
+  </si>
+  <si>
+    <t>Timer B 0 out H</t>
+  </si>
+  <si>
+    <t>CPU Status Register Bit SCG1</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>PJ.1</t>
+  </si>
+  <si>
+    <t>Master Clock</t>
+  </si>
+  <si>
+    <t>CPU Status Register Bit SCG0</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>PJ.2</t>
+  </si>
+  <si>
+    <t>Auxilary Clock</t>
+  </si>
+  <si>
+    <t>CPU Status Register Bit OSCOFF</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>PJ.3</t>
+  </si>
+  <si>
+    <t>CPU Status Register Bit CPUOFF</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>PJ.4</t>
+  </si>
+  <si>
+    <t>Low Freq Crystal Input</t>
+  </si>
+  <si>
+    <t>PJ.5</t>
+  </si>
+  <si>
+    <t>Low Freq Crystal Output</t>
+  </si>
+  <si>
+    <t>PJ.6</t>
+  </si>
+  <si>
+    <t>High Freq Crystal Input</t>
+  </si>
+  <si>
+    <t>PJ.7</t>
+  </si>
+  <si>
+    <t>High Freq Crystal Output</t>
   </si>
 </sst>
 </file>
@@ -314,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +393,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,11 +424,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E145" sqref="E130:E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -680,6 +756,7 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="6" max="6" width="93" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1005,7 +1082,7 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -1038,13 +1115,13 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C33" t="s">
         <v>47</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2120,7 +2197,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="129" spans="2:4">
+    <row r="129" spans="1:5">
       <c r="B129" t="s">
         <v>12</v>
       </c>
@@ -2129,6 +2206,398 @@
       </c>
       <c r="D129" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>92</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C130" t="s">
+        <v>6</v>
+      </c>
+      <c r="D130" t="s">
+        <v>6</v>
+      </c>
+      <c r="E130" s="4"/>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="B131" t="s">
+        <v>7</v>
+      </c>
+      <c r="C131" t="s">
+        <v>93</v>
+      </c>
+      <c r="D131" t="s">
+        <v>78</v>
+      </c>
+      <c r="E131" s="4"/>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="B132" t="s">
+        <v>10</v>
+      </c>
+      <c r="C132" t="s">
+        <v>59</v>
+      </c>
+      <c r="D132" t="s">
+        <v>94</v>
+      </c>
+      <c r="E132" s="4"/>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="B133" t="s">
+        <v>12</v>
+      </c>
+      <c r="C133" t="s">
+        <v>62</v>
+      </c>
+      <c r="D133" t="s">
+        <v>95</v>
+      </c>
+      <c r="E133" s="4"/>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>96</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C134" t="s">
+        <v>6</v>
+      </c>
+      <c r="D134" t="s">
+        <v>6</v>
+      </c>
+      <c r="E134" s="4"/>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="B135" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" t="s">
+        <v>59</v>
+      </c>
+      <c r="D135" t="s">
+        <v>97</v>
+      </c>
+      <c r="E135" s="4"/>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="B136" t="s">
+        <v>10</v>
+      </c>
+      <c r="C136" t="s">
+        <v>59</v>
+      </c>
+      <c r="D136" t="s">
+        <v>98</v>
+      </c>
+      <c r="E136" s="4"/>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="B137" t="s">
+        <v>12</v>
+      </c>
+      <c r="C137" t="s">
+        <v>62</v>
+      </c>
+      <c r="D137" t="s">
+        <v>99</v>
+      </c>
+      <c r="E137" s="4"/>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>100</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138" t="s">
+        <v>6</v>
+      </c>
+      <c r="E138" s="4"/>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="B139" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139" t="s">
+        <v>59</v>
+      </c>
+      <c r="D139" t="s">
+        <v>101</v>
+      </c>
+      <c r="E139" s="4"/>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="B140" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" t="s">
+        <v>59</v>
+      </c>
+      <c r="D140" t="s">
+        <v>102</v>
+      </c>
+      <c r="E140" s="4"/>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="B141" t="s">
+        <v>12</v>
+      </c>
+      <c r="C141" t="s">
+        <v>62</v>
+      </c>
+      <c r="D141" t="s">
+        <v>103</v>
+      </c>
+      <c r="E141" s="4"/>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
+        <v>104</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142" t="s">
+        <v>6</v>
+      </c>
+      <c r="D142" t="s">
+        <v>6</v>
+      </c>
+      <c r="E142" s="4"/>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="B143" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" t="s">
+        <v>59</v>
+      </c>
+      <c r="D143" t="s">
+        <v>62</v>
+      </c>
+      <c r="E143" s="4"/>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" t="s">
+        <v>59</v>
+      </c>
+      <c r="D144" t="s">
+        <v>105</v>
+      </c>
+      <c r="E144" s="4"/>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="B145" t="s">
+        <v>12</v>
+      </c>
+      <c r="C145" t="s">
+        <v>62</v>
+      </c>
+      <c r="D145" t="s">
+        <v>106</v>
+      </c>
+      <c r="E145" s="4"/>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" t="s">
+        <v>6</v>
+      </c>
+      <c r="D146" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="B147" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D147" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="B148" t="s">
+        <v>10</v>
+      </c>
+      <c r="C148" t="s">
+        <v>59</v>
+      </c>
+      <c r="D148" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="B149" t="s">
+        <v>12</v>
+      </c>
+      <c r="C149" t="s">
+        <v>59</v>
+      </c>
+      <c r="D149" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150" t="s">
+        <v>6</v>
+      </c>
+      <c r="D150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="B151" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D151" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="B152" t="s">
+        <v>10</v>
+      </c>
+      <c r="C152" t="s">
+        <v>59</v>
+      </c>
+      <c r="D152" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="B153" t="s">
+        <v>12</v>
+      </c>
+      <c r="C153" t="s">
+        <v>59</v>
+      </c>
+      <c r="D153" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" t="s">
+        <v>111</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154" t="s">
+        <v>6</v>
+      </c>
+      <c r="D154" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="B155" t="s">
+        <v>7</v>
+      </c>
+      <c r="C155" t="s">
+        <v>112</v>
+      </c>
+      <c r="D155" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="B156" t="s">
+        <v>10</v>
+      </c>
+      <c r="C156" t="s">
+        <v>59</v>
+      </c>
+      <c r="D156" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="B157" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" t="s">
+        <v>59</v>
+      </c>
+      <c r="D157" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" t="s">
+        <v>113</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C158" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="B159" t="s">
+        <v>7</v>
+      </c>
+      <c r="C159" t="s">
+        <v>114</v>
+      </c>
+      <c r="D159" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="B160" t="s">
+        <v>10</v>
+      </c>
+      <c r="C160" t="s">
+        <v>59</v>
+      </c>
+      <c r="D160" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4">
+      <c r="B161" t="s">
+        <v>12</v>
+      </c>
+      <c r="C161" t="s">
+        <v>59</v>
+      </c>
+      <c r="D161" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I changed all the files listed mainly so it would build correctly with TI's compiler. Also Changed some stuff in the GPIO pin document shwoing that we are using the UART pins and leaving a note detailing which pins are used for SPI so they can be used if needed. Finally Got a new copy of the BSL manual because the other copy of the PDF wasnt working for some reason. Opens now so should be all good.
</commit_message>
<xml_diff>
--- a/docs/GPIOalternateFunctionList.xlsx
+++ b/docs/GPIOalternateFunctionList.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21506"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21513"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="480" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{622749EB-DCF6-4A66-B22A-7F7CAC1B9150}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B65EB4A0-86BB-4D94-A1E8-1598CE740ECB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="131">
   <si>
     <t>Pin</t>
   </si>
@@ -64,7 +64,7 @@
     <t>TIRTIARY</t>
   </si>
   <si>
-    <t>Analog Setting</t>
+    <t>Analog Setting A0</t>
   </si>
   <si>
     <t>P1.1</t>
@@ -85,6 +85,9 @@
     <t>COUT</t>
   </si>
   <si>
+    <t>Analog Setting A1</t>
+  </si>
+  <si>
     <t>P1.2</t>
   </si>
   <si>
@@ -97,6 +100,9 @@
     <t>Timer A 0 CLK</t>
   </si>
   <si>
+    <t>Analog Setting A2</t>
+  </si>
+  <si>
     <t>P1.3</t>
   </si>
   <si>
@@ -109,6 +115,9 @@
     <t>eUSCI A SPI mode Slave Transmit Enable</t>
   </si>
   <si>
+    <t>Analog Setting A3</t>
+  </si>
+  <si>
     <t>P1.4</t>
   </si>
   <si>
@@ -121,6 +130,9 @@
     <t>eUSCI B SPI mode Slave Transmit Enable</t>
   </si>
   <si>
+    <t>Analog Setting A4</t>
+  </si>
+  <si>
     <t>P1.5</t>
   </si>
   <si>
@@ -133,7 +145,7 @@
     <t>eUSCI A SPI mode CLK</t>
   </si>
   <si>
-    <t xml:space="preserve"> Analog Setting</t>
+    <t> Analog Setting A5</t>
   </si>
   <si>
     <t>P1.6</t>
@@ -220,12 +232,21 @@
     <t>Timer A 0 Capture and compare input 0</t>
   </si>
   <si>
+    <t>Analog Setting A6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should probably be saved in case an SPI signal is needed. </t>
+  </si>
+  <si>
     <t>P2.4</t>
   </si>
   <si>
     <t>Timer A 1 Channel 0</t>
   </si>
   <si>
+    <t>Analog Setting A7</t>
+  </si>
+  <si>
     <t>P2.5</t>
   </si>
   <si>
@@ -244,15 +265,27 @@
     <t>P3.0</t>
   </si>
   <si>
+    <t>Analog Setting A12</t>
+  </si>
+  <si>
     <t>P3.1</t>
   </si>
   <si>
+    <t>Analog Setting A13</t>
+  </si>
+  <si>
     <t>P3.2</t>
   </si>
   <si>
+    <t>Analog Setting A14</t>
+  </si>
+  <si>
     <t>P3.3</t>
   </si>
   <si>
+    <t>Analog Setting A15</t>
+  </si>
+  <si>
     <t>P3.4</t>
   </si>
   <si>
@@ -280,15 +313,27 @@
     <t>P4.0</t>
   </si>
   <si>
+    <t>Analog Setting A8</t>
+  </si>
+  <si>
     <t>P4.1</t>
   </si>
   <si>
+    <t>Analog Setting A9</t>
+  </si>
+  <si>
     <t>P4.2</t>
   </si>
   <si>
+    <t>Analog Setting A10</t>
+  </si>
+  <si>
     <t>P4.3</t>
   </si>
   <si>
+    <t>Analog Setting A11</t>
+  </si>
+  <si>
     <t>P4.4</t>
   </si>
   <si>
@@ -302,6 +347,9 @@
   </si>
   <si>
     <t>PJ.0</t>
+  </si>
+  <si>
+    <t>Pins J0-3 are shared with the 4 pin Jtag and if jtag is selected then none of the functions listed are available.</t>
   </si>
   <si>
     <t>Timer B 0 out H</t>
@@ -383,7 +431,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +447,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF70AD47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,12 +478,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E145" sqref="E130:E145"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -861,12 +916,12 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
@@ -883,10 +938,10 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -894,7 +949,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
@@ -905,12 +960,12 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>5</v>
@@ -927,10 +982,10 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -938,7 +993,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -949,12 +1004,12 @@
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>5</v>
@@ -971,10 +1026,10 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -982,7 +1037,7 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -993,12 +1048,12 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
@@ -1015,10 +1070,10 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1026,7 +1081,7 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1034,12 +1089,12 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -1056,10 +1111,10 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1067,7 +1122,7 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1075,15 +1130,15 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1100,10 +1155,10 @@
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1111,331 +1166,350 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="B36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="B40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="B33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="B37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D51" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="B41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>59</v>
-      </c>
-      <c r="D43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="B45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>27</v>
-      </c>
-      <c r="D48" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="B49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
-        <v>47</v>
-      </c>
-      <c r="D51" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="B52" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="B53" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="B55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="B56" t="s">
-        <v>10</v>
-      </c>
-      <c r="C56" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="B57" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="B59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s">
-        <v>59</v>
-      </c>
-      <c r="D59" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="B60" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="1:6">
       <c r="B61" t="s">
         <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D61" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>66</v>
+      </c>
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>5</v>
@@ -1447,26 +1521,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:6">
       <c r="B63" t="s">
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D63" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="B64" t="s">
         <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1474,15 +1548,15 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D65" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>5</v>
@@ -1499,10 +1573,10 @@
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D67" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1510,10 +1584,10 @@
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D68" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1521,12 +1595,12 @@
         <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="3" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>5</v>
@@ -1543,10 +1617,10 @@
         <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D71" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1554,10 +1628,10 @@
         <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D72" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1565,12 +1639,12 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>5</v>
@@ -1587,10 +1661,10 @@
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D75" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1598,10 +1672,10 @@
         <v>10</v>
       </c>
       <c r="C76" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D76" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1609,12 +1683,12 @@
         <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>5</v>
@@ -1631,10 +1705,10 @@
         <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D79" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1642,10 +1716,10 @@
         <v>10</v>
       </c>
       <c r="C80" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D80" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1653,12 +1727,12 @@
         <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>5</v>
@@ -1675,10 +1749,10 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D83" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1686,10 +1760,10 @@
         <v>10</v>
       </c>
       <c r="C84" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D84" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1697,15 +1771,15 @@
         <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D85" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="3" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>5</v>
@@ -1722,10 +1796,10 @@
         <v>7</v>
       </c>
       <c r="C87" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D87" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1733,7 +1807,7 @@
         <v>10</v>
       </c>
       <c r="C88" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D88" t="s">
         <v>19</v>
@@ -1744,15 +1818,15 @@
         <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D89" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="3" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>5</v>
@@ -1769,10 +1843,10 @@
         <v>7</v>
       </c>
       <c r="C91" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="D91" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1780,10 +1854,10 @@
         <v>10</v>
       </c>
       <c r="C92" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D92" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1791,15 +1865,15 @@
         <v>12</v>
       </c>
       <c r="C93" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D93" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="3" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>5</v>
@@ -1816,10 +1890,10 @@
         <v>7</v>
       </c>
       <c r="C95" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D95" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1827,10 +1901,10 @@
         <v>10</v>
       </c>
       <c r="C96" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D96" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1838,15 +1912,15 @@
         <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D97" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="3" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>5</v>
@@ -1863,10 +1937,10 @@
         <v>7</v>
       </c>
       <c r="C99" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D99" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1874,10 +1948,10 @@
         <v>10</v>
       </c>
       <c r="C100" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D100" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1885,12 +1959,12 @@
         <v>12</v>
       </c>
       <c r="C101" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="3" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>5</v>
@@ -1907,10 +1981,10 @@
         <v>7</v>
       </c>
       <c r="C103" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D103" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1918,10 +1992,10 @@
         <v>10</v>
       </c>
       <c r="C104" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D104" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1929,12 +2003,12 @@
         <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>5</v>
@@ -1951,10 +2025,10 @@
         <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D107" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1962,10 +2036,10 @@
         <v>10</v>
       </c>
       <c r="C108" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D108" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1973,12 +2047,12 @@
         <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>5</v>
@@ -1995,10 +2069,10 @@
         <v>7</v>
       </c>
       <c r="C111" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D111" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2006,10 +2080,10 @@
         <v>10</v>
       </c>
       <c r="C112" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D112" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2017,12 +2091,12 @@
         <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="3" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>5</v>
@@ -2039,10 +2113,10 @@
         <v>7</v>
       </c>
       <c r="C115" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="D115" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2050,10 +2124,10 @@
         <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D116" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2061,15 +2135,15 @@
         <v>12</v>
       </c>
       <c r="C117" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D117" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="3" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>5</v>
@@ -2086,10 +2160,10 @@
         <v>7</v>
       </c>
       <c r="C119" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D119" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2097,10 +2171,10 @@
         <v>10</v>
       </c>
       <c r="C120" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D120" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2108,15 +2182,15 @@
         <v>12</v>
       </c>
       <c r="C121" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D121" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="3" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>5</v>
@@ -2133,10 +2207,10 @@
         <v>7</v>
       </c>
       <c r="C123" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D123" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2144,10 +2218,10 @@
         <v>10</v>
       </c>
       <c r="C124" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D124" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2155,15 +2229,15 @@
         <v>12</v>
       </c>
       <c r="C125" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D125" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="3" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>5</v>
@@ -2180,10 +2254,10 @@
         <v>7</v>
       </c>
       <c r="C127" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D127" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2191,26 +2265,26 @@
         <v>10</v>
       </c>
       <c r="C128" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D128" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="B129" t="s">
         <v>12</v>
       </c>
       <c r="C129" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D129" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>5</v>
@@ -2222,46 +2296,49 @@
         <v>6</v>
       </c>
       <c r="E130" s="4"/>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="B131" t="s">
         <v>7</v>
       </c>
       <c r="C131" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="D131" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:6">
       <c r="B132" t="s">
         <v>10</v>
       </c>
       <c r="C132" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D132" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:6">
       <c r="B133" t="s">
         <v>12</v>
       </c>
       <c r="C133" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D133" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>5</v>
@@ -2274,45 +2351,45 @@
       </c>
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:6">
       <c r="B135" t="s">
         <v>7</v>
       </c>
       <c r="C135" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D135" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:6">
       <c r="B136" t="s">
         <v>10</v>
       </c>
       <c r="C136" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D136" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:6">
       <c r="B137" t="s">
         <v>12</v>
       </c>
       <c r="C137" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D137" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>5</v>
@@ -2325,45 +2402,45 @@
       </c>
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:6">
       <c r="B139" t="s">
         <v>7</v>
       </c>
       <c r="C139" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D139" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:6">
       <c r="B140" t="s">
         <v>10</v>
       </c>
       <c r="C140" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D140" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:6">
       <c r="B141" t="s">
         <v>12</v>
       </c>
       <c r="C141" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D141" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>5</v>
@@ -2376,27 +2453,27 @@
       </c>
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:6">
       <c r="B143" t="s">
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D143" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:6">
       <c r="B144" t="s">
         <v>10</v>
       </c>
       <c r="C144" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D144" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="E144" s="4"/>
     </row>
@@ -2405,16 +2482,16 @@
         <v>12</v>
       </c>
       <c r="C145" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D145" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="E145" s="4"/>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="1" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>5</v>
@@ -2431,10 +2508,10 @@
         <v>7</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D147" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -2442,10 +2519,10 @@
         <v>10</v>
       </c>
       <c r="C148" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D148" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -2453,15 +2530,15 @@
         <v>12</v>
       </c>
       <c r="C149" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D149" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="1" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>5</v>
@@ -2478,10 +2555,10 @@
         <v>7</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="D151" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -2489,10 +2566,10 @@
         <v>10</v>
       </c>
       <c r="C152" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D152" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -2500,15 +2577,15 @@
         <v>12</v>
       </c>
       <c r="C153" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D153" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>5</v>
@@ -2525,10 +2602,10 @@
         <v>7</v>
       </c>
       <c r="C155" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="D155" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -2536,10 +2613,10 @@
         <v>10</v>
       </c>
       <c r="C156" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D156" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -2547,15 +2624,15 @@
         <v>12</v>
       </c>
       <c r="C157" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D157" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>5</v>
@@ -2572,10 +2649,10 @@
         <v>7</v>
       </c>
       <c r="C159" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="D159" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -2583,10 +2660,10 @@
         <v>10</v>
       </c>
       <c r="C160" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D160" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="161" spans="2:4">
@@ -2594,10 +2671,10 @@
         <v>12</v>
       </c>
       <c r="C161" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D161" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>